<commit_message>
TP4 - Final arternativo Nro5 - El despertar del Grafo
</commit_message>
<xml_diff>
--- a/Estadisticas/Grafos Aleatorios.xlsx
+++ b/Estadisticas/Grafos Aleatorios.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tekno\Desktop\Repositorio\TP4-ColoreoDeGrafos\Estadisticas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="30" windowWidth="6915" windowHeight="7995"/>
   </bookViews>
@@ -47,8 +42,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,27 +117,17 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="142"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="42"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-AR"/>
+  <c:style val="42"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.1088667051581355E-2"/>
+          <c:x val="5.1088667051581375E-2"/>
           <c:y val="2.6600823330968221E-2"/>
           <c:w val="0.81195370262022581"/>
           <c:h val="0.944612538186825"/>
@@ -150,7 +135,6 @@
       </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -270,8 +254,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E944-46C4-BCB6-76B2EB33DF24}"/>
             </c:ext>
@@ -396,8 +379,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-E944-46C4-BCB6-76B2EB33DF24}"/>
             </c:ext>
@@ -522,57 +504,42 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-E944-46C4-BCB6-76B2EB33DF24}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="75022720"/>
-        <c:axId val="75024256"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="98292864"/>
+        <c:axId val="98294400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75022720"/>
+        <c:axId val="98292864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75024256"/>
+        <c:crossAx val="98294400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75024256"/>
+        <c:axId val="98294400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3800"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75022720"/>
+        <c:crossAx val="98292864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -585,44 +552,31 @@
           <c:yMode val="edge"/>
           <c:x val="0.86350687312736529"/>
           <c:y val="0.44071167333591488"/>
-          <c:w val="0.13649312687263468"/>
-          <c:h val="0.11857648121853621"/>
+          <c:w val="0.13649312687263473"/>
+          <c:h val="0.11857648121853623"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="142"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="42"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-AR"/>
+  <c:style val="42"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -778,8 +732,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-364C-4E08-9919-168C5CBFB21E}"/>
             </c:ext>
@@ -940,8 +893,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-364C-4E08-9919-168C5CBFB21E}"/>
             </c:ext>
@@ -1102,97 +1054,69 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-364C-4E08-9919-168C5CBFB21E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="76000640"/>
-        <c:axId val="76027008"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="98212096"/>
+        <c:axId val="98230272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76000640"/>
+        <c:axId val="98212096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76027008"/>
+        <c:crossAx val="98230272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76027008"/>
+        <c:axId val="98230272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3500"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76000640"/>
+        <c:crossAx val="98212096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="142"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="42"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-AR"/>
+  <c:style val="42"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1426,8 +1350,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3701-4649-AE33-D57620A56242}"/>
             </c:ext>
@@ -1666,8 +1589,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3701-4649-AE33-D57620A56242}"/>
             </c:ext>
@@ -1906,72 +1828,55 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-3701-4649-AE33-D57620A56242}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="76061312"/>
-        <c:axId val="76079488"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="98384896"/>
+        <c:axId val="98403072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76061312"/>
+        <c:axId val="98384896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76079488"/>
+        <c:crossAx val="98403072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76079488"/>
+        <c:axId val="98403072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1900"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76061312"/>
+        <c:crossAx val="98384896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1997,7 +1902,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2038,7 +1943,7 @@
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2079,7 +1984,7 @@
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2143,7 +2048,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2175,27 +2080,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2227,24 +2114,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2420,14 +2289,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
@@ -2435,7 +2304,7 @@
     <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2444,13 +2313,13 @@
       <c r="D1" s="5"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -2464,7 +2333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>61</v>
       </c>
@@ -2478,7 +2347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>62</v>
       </c>
@@ -2492,7 +2361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>63</v>
       </c>
@@ -2506,7 +2375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>64</v>
       </c>
@@ -2520,7 +2389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>65</v>
       </c>
@@ -2534,7 +2403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>66</v>
       </c>
@@ -2548,7 +2417,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>67</v>
       </c>
@@ -2562,7 +2431,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>68</v>
       </c>
@@ -2576,7 +2445,7 @@
         <v>1709</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>69</v>
       </c>
@@ -2590,7 +2459,7 @@
         <v>3379</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>70</v>
       </c>
@@ -2604,7 +2473,7 @@
         <v>2931</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>71</v>
       </c>
@@ -2618,7 +2487,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>72</v>
       </c>
@@ -2632,7 +2501,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>73</v>
       </c>
@@ -2646,7 +2515,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>74</v>
       </c>
@@ -2660,7 +2529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <f>SUM(B4:B17)</f>
@@ -2675,31 +2544,31 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2715,14 +2584,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D24" sqref="B24:D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
@@ -2730,7 +2599,7 @@
     <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -2739,13 +2608,13 @@
       <c r="D1" s="5"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -2759,7 +2628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>94</v>
       </c>
@@ -2773,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>95</v>
       </c>
@@ -2787,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>96</v>
       </c>
@@ -2801,7 +2670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>97</v>
       </c>
@@ -2815,7 +2684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="2">
         <v>98</v>
       </c>
@@ -2829,7 +2698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>99</v>
       </c>
@@ -2843,7 +2712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>100</v>
       </c>
@@ -2857,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>101</v>
       </c>
@@ -2871,7 +2740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>102</v>
       </c>
@@ -2885,7 +2754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>103</v>
       </c>
@@ -2899,7 +2768,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>104</v>
       </c>
@@ -2913,7 +2782,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>105</v>
       </c>
@@ -2927,7 +2796,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>106</v>
       </c>
@@ -2941,7 +2810,7 @@
         <v>1687</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>107</v>
       </c>
@@ -2955,7 +2824,7 @@
         <v>2554</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>108</v>
       </c>
@@ -2969,7 +2838,7 @@
         <v>2375</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>109</v>
       </c>
@@ -2983,7 +2852,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>110</v>
       </c>
@@ -2997,7 +2866,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>111</v>
       </c>
@@ -3011,7 +2880,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>112</v>
       </c>
@@ -3025,7 +2894,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>113</v>
       </c>
@@ -3039,7 +2908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="B24">
         <f>SUM(B4:B23)</f>
         <v>10000</v>
@@ -3053,31 +2922,31 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
@@ -3093,14 +2962,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
@@ -3108,7 +2977,7 @@
     <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -3117,13 +2986,13 @@
       <c r="D1" s="5"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -3137,7 +3006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>192</v>
       </c>
@@ -3151,7 +3020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>193</v>
       </c>
@@ -3165,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>194</v>
       </c>
@@ -3179,7 +3048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>195</v>
       </c>
@@ -3193,7 +3062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="2">
         <v>196</v>
       </c>
@@ -3207,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="2">
         <v>197</v>
       </c>
@@ -3221,7 +3090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="2">
         <v>198</v>
       </c>
@@ -3235,7 +3104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="2">
         <v>199</v>
       </c>
@@ -3249,7 +3118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>200</v>
       </c>
@@ -3263,7 +3132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>201</v>
       </c>
@@ -3277,7 +3146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>202</v>
       </c>
@@ -3291,7 +3160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>203</v>
       </c>
@@ -3305,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>204</v>
       </c>
@@ -3319,7 +3188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>205</v>
       </c>
@@ -3333,7 +3202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>206</v>
       </c>
@@ -3347,7 +3216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>207</v>
       </c>
@@ -3361,7 +3230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>208</v>
       </c>
@@ -3375,7 +3244,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>209</v>
       </c>
@@ -3389,7 +3258,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>210</v>
       </c>
@@ -3403,7 +3272,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>211</v>
       </c>
@@ -3417,7 +3286,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>212</v>
       </c>
@@ -3431,7 +3300,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="1">
         <v>213</v>
       </c>
@@ -3445,7 +3314,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="1">
         <v>214</v>
       </c>
@@ -3459,7 +3328,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="1">
         <v>215</v>
       </c>
@@ -3473,7 +3342,7 @@
         <v>1563</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="1">
         <v>216</v>
       </c>
@@ -3487,7 +3356,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="1">
         <v>217</v>
       </c>
@@ -3501,7 +3370,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>218</v>
       </c>
@@ -3515,7 +3384,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="1">
         <v>219</v>
       </c>
@@ -3529,7 +3398,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="1">
         <v>220</v>
       </c>
@@ -3543,7 +3412,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" s="1">
         <v>221</v>
       </c>
@@ -3557,7 +3426,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="1">
         <v>222</v>
       </c>
@@ -3571,7 +3440,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="1">
         <v>223</v>
       </c>
@@ -3585,7 +3454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="1">
         <v>224</v>
       </c>
@@ -3599,7 +3468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="B37">
         <f>SUM(B4:B36)</f>
         <v>10000</v>
@@ -3613,19 +3482,19 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>

</xml_diff>

<commit_message>
TP4 - Final alternativo Nro6 - El Señor de los Grafos: Los dos Nodos
</commit_message>
<xml_diff>
--- a/Estadisticas/Grafos Aleatorios.xlsx
+++ b/Estadisticas/Grafos Aleatorios.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="6915" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="6915" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="600y40" sheetId="1" r:id="rId1"/>
     <sheet name="600y60" sheetId="3" r:id="rId2"/>
     <sheet name="600y90" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Estadistica Grafo Aleatorio 600 Nodos y 40% Ady</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>Secuencial aleatorio</t>
+  </si>
+  <si>
+    <t>Frec. Rel SA</t>
+  </si>
+  <si>
+    <t>Sec. Rel. WP</t>
+  </si>
+  <si>
+    <t>Sec. Rel. M</t>
   </si>
 </sst>
 </file>
@@ -84,7 +93,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -96,6 +105,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -127,7 +139,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.1088667051581375E-2"/>
+          <c:x val="5.1088667051581396E-2"/>
           <c:y val="2.6600823330968221E-2"/>
           <c:w val="0.81195370262022581"/>
           <c:h val="0.944612538186825"/>
@@ -510,27 +522,26 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="98292864"/>
-        <c:axId val="98294400"/>
+        <c:axId val="114390912"/>
+        <c:axId val="114392448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98292864"/>
+        <c:axId val="114390912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98294400"/>
+        <c:crossAx val="114392448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98294400"/>
+        <c:axId val="114392448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3800"/>
@@ -539,7 +550,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98292864"/>
+        <c:crossAx val="114390912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -552,8 +563,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.86350687312736529"/>
           <c:y val="0.44071167333591488"/>
-          <c:w val="0.13649312687263473"/>
-          <c:h val="0.11857648121853623"/>
+          <c:w val="0.13649312687263476"/>
+          <c:h val="0.11857648121853624"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -562,7 +573,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1060,27 +1071,26 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="98212096"/>
-        <c:axId val="98230272"/>
+        <c:axId val="77331456"/>
+        <c:axId val="114696960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98212096"/>
+        <c:axId val="77331456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98230272"/>
+        <c:crossAx val="114696960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98230272"/>
+        <c:axId val="114696960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3500"/>
@@ -1089,20 +1099,21 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98212096"/>
+        <c:crossAx val="77331456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1361,7 +1372,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'600y90'!$C$3</c:f>
+              <c:f>'600y90'!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1483,7 +1494,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'600y90'!$C$4:$C$36</c:f>
+              <c:f>'600y90'!$D$4:$D$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
@@ -1600,7 +1611,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'600y90'!$D$3</c:f>
+              <c:f>'600y90'!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1722,7 +1733,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'600y90'!$D$4:$D$36</c:f>
+              <c:f>'600y90'!$F$4:$F$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
@@ -1834,27 +1845,26 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="98384896"/>
-        <c:axId val="98403072"/>
+        <c:axId val="114770304"/>
+        <c:axId val="114771840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98384896"/>
+        <c:axId val="114770304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98403072"/>
+        <c:crossAx val="114771840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98403072"/>
+        <c:axId val="114771840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1900"/>
@@ -1863,20 +1873,791 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98384896"/>
+        <c:crossAx val="114770304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-AR"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR"/>
+              <a:t>Gráfico</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-AR" baseline="0"/>
+              <a:t> de frecuencia relativa</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'600y90'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Frec. Rel SA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'600y90'!$A$4:$A$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>224</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'600y90'!$C$4:$C$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.8E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.8999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.8700000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0599999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.1400000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.105</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.13420000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15279999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.15260000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.1249</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.5199999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.2200000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.9399999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.5599999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.4999999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.6999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6.9999999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'600y90'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sec. Rel. WP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'600y90'!$A$4:$A$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>224</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'600y90'!$E$4:$E$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9100000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.2799999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15679999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.16550000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.17349999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.15229999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1196</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.45E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4899999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.1999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.6999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.9999999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'600y90'!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sec. Rel. M</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'600y90'!$A$4:$A$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>224</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'600y90'!$G$4:$G$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.9999999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.1000000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.1900000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.63E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.5199999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.2799999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.1255</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.1575</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.15629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.1416</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.1084</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.7299999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.5999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.72E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.7000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8.9999999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="131513344"/>
+        <c:axId val="131535616"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="131513344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="131535616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="131535616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="131513344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1887,22 +2668,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1943,7 +2724,7 @@
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1969,22 +2750,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
+      <xdr:colOff>159204</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>68035</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1997,6 +2778,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>394606</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>122464</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>625928</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="3 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2292,7 +3103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -2305,19 +3116,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
@@ -2587,7 +3398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="D24" sqref="B24:D24"/>
     </sheetView>
   </sheetViews>
@@ -2600,19 +3411,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
@@ -2963,36 +3774,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -3000,13 +3820,22 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="G3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2">
         <v>192</v>
       </c>
@@ -3014,13 +3843,25 @@
         <v>0</v>
       </c>
       <c r="C4" s="2">
+        <f>B4/10000</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
         <v>2</v>
       </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" s="2">
+        <f>D4/10000</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <f>F4/10000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="2">
         <v>193</v>
       </c>
@@ -3028,13 +3869,25 @@
         <v>0</v>
       </c>
       <c r="C5" s="2">
+        <f t="shared" ref="C5:C36" si="0">B5/10000</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
         <v>15</v>
       </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:E36" si="1">D5/10000</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G36" si="2">F5/10000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="2">
         <v>194</v>
       </c>
@@ -3042,13 +3895,25 @@
         <v>0</v>
       </c>
       <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
         <v>52</v>
       </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6" s="2">
+        <f t="shared" si="1"/>
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="2">
         <v>195</v>
       </c>
@@ -3056,13 +3921,25 @@
         <v>0</v>
       </c>
       <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
         <v>142</v>
       </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="2">
         <v>196</v>
       </c>
@@ -3070,13 +3947,25 @@
         <v>0</v>
       </c>
       <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
         <v>391</v>
       </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>3.9100000000000003E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="2">
         <v>197</v>
       </c>
@@ -3084,27 +3973,51 @@
         <v>1</v>
       </c>
       <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+      <c r="D9" s="2">
         <v>828</v>
       </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>8.2799999999999999E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="2">
         <v>198</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+      <c r="D10" s="1">
         <v>1568</v>
       </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.15679999999999999</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2">
         <v>199</v>
       </c>
@@ -3112,13 +4025,25 @@
         <v>5</v>
       </c>
       <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D11" s="2">
         <v>1655</v>
       </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16550000000000001</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>200</v>
       </c>
@@ -3126,383 +4051,692 @@
         <v>28</v>
       </c>
       <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>2.8E-3</v>
+      </c>
+      <c r="D12" s="2">
         <v>1735</v>
       </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.17349999999999999</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>201</v>
       </c>
       <c r="B13" s="1">
         <v>69</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="D13" s="1">
         <v>1523</v>
       </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.15229999999999999</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>202</v>
       </c>
       <c r="B14" s="1">
         <v>187</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="D14" s="1">
         <v>1196</v>
       </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="E14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.1196</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>203</v>
       </c>
       <c r="B15" s="1">
         <v>406</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>4.0599999999999997E-2</v>
+      </c>
+      <c r="D15" s="1">
         <v>545</v>
       </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>5.45E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>204</v>
       </c>
       <c r="B16" s="1">
         <v>714</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="D16" s="1">
         <v>249</v>
       </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>2.4899999999999999E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>205</v>
       </c>
       <c r="B17" s="1">
         <v>1050</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.105</v>
+      </c>
+      <c r="D17" s="1">
         <v>72</v>
       </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="2">
+        <f t="shared" si="1"/>
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>206</v>
       </c>
       <c r="B18" s="1">
         <v>1342</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13420000000000001</v>
+      </c>
+      <c r="D18" s="1">
         <v>17</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="F18" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="G18" s="2">
+        <f t="shared" si="2"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>207</v>
       </c>
       <c r="B19" s="1">
         <v>1528</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15279999999999999</v>
+      </c>
+      <c r="D19" s="1">
         <v>9</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="2">
+        <f t="shared" si="1"/>
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="F19" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="G19" s="2">
+        <f t="shared" si="2"/>
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>208</v>
       </c>
       <c r="B20" s="1">
         <v>1526</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15260000000000001</v>
+      </c>
+      <c r="D20" s="1">
         <v>1</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
+        <v>1E-4</v>
+      </c>
+      <c r="F20" s="1">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="G20" s="2">
+        <f t="shared" si="2"/>
+        <v>4.1000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>209</v>
       </c>
       <c r="B21" s="1">
         <v>1249</v>
       </c>
-      <c r="C21" s="1">
-        <v>0</v>
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1249</v>
       </c>
       <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
         <v>119</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="G21" s="2">
+        <f t="shared" si="2"/>
+        <v>1.1900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>210</v>
       </c>
       <c r="B22" s="1">
         <v>852</v>
       </c>
-      <c r="C22" s="1">
-        <v>0</v>
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>8.5199999999999998E-2</v>
       </c>
       <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
         <v>263</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="G22" s="2">
+        <f t="shared" si="2"/>
+        <v>2.63E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>211</v>
       </c>
       <c r="B23" s="1">
         <v>522</v>
       </c>
-      <c r="C23" s="1">
-        <v>0</v>
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>5.2200000000000003E-2</v>
       </c>
       <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
         <v>552</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="G23" s="2">
+        <f t="shared" si="2"/>
+        <v>5.5199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>212</v>
       </c>
       <c r="B24" s="1">
         <v>294</v>
       </c>
-      <c r="C24" s="1">
-        <v>0</v>
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>2.9399999999999999E-2</v>
       </c>
       <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
         <v>828</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="G24" s="2">
+        <f t="shared" si="2"/>
+        <v>8.2799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>213</v>
       </c>
       <c r="B25" s="1">
         <v>156</v>
       </c>
-      <c r="C25" s="1">
-        <v>0</v>
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5599999999999999E-2</v>
       </c>
       <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
         <v>1255</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="G25" s="2">
+        <f>F25/10000</f>
+        <v>0.1255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>214</v>
       </c>
       <c r="B26" s="1">
         <v>45</v>
       </c>
-      <c r="C26" s="1">
-        <v>0</v>
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
         <v>1575</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="G26" s="2">
+        <f t="shared" si="2"/>
+        <v>0.1575</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
         <v>215</v>
       </c>
       <c r="B27" s="1">
         <v>17</v>
       </c>
-      <c r="C27" s="1">
-        <v>0</v>
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
         <v>1563</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="G27" s="2">
+        <f t="shared" si="2"/>
+        <v>0.15629999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>216</v>
       </c>
       <c r="B28" s="1">
         <v>7</v>
       </c>
-      <c r="C28" s="1">
-        <v>0</v>
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
         <v>1416</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="G28" s="2">
+        <f t="shared" si="2"/>
+        <v>0.1416</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>217</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
       </c>
-      <c r="C29" s="1">
-        <v>0</v>
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
       </c>
       <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
         <v>1084</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="G29" s="2">
+        <f t="shared" si="2"/>
+        <v>0.1084</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="1">
         <v>218</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
         <v>673</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="G30" s="2">
+        <f t="shared" si="2"/>
+        <v>6.7299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="1">
         <v>219</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
         <v>360</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="G31" s="2">
+        <f t="shared" si="2"/>
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>220</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
         <v>172</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="G32" s="2">
+        <f t="shared" si="2"/>
+        <v>1.72E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="1">
         <v>221</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
         <v>57</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="G33" s="2">
+        <f t="shared" si="2"/>
+        <v>5.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="1">
         <v>222</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="G34" s="2">
+        <f t="shared" si="2"/>
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="1">
         <v>223</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="G35" s="2">
+        <f t="shared" si="2"/>
+        <v>8.9999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="1">
         <v>224</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="G36" s="2">
+        <f t="shared" si="2"/>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="B37">
         <f>SUM(B4:B36)</f>
         <v>10000</v>
       </c>
-      <c r="C37">
-        <f t="shared" ref="C37:D37" si="0">SUM(C4:C36)</f>
+      <c r="D37">
+        <f t="shared" ref="D37:F37" si="3">SUM(D4:D36)</f>
         <v>10000</v>
       </c>
-      <c r="D37">
-        <f t="shared" si="0"/>
+      <c r="F37">
+        <f t="shared" si="3"/>
         <v>10000</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:7">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="A1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>